<commit_message>
Automatische test-sync: 2025-07-29 21:35:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Inhoud</t>
   </si>
@@ -22,6 +22,30 @@
     <t>Antwoord</t>
   </si>
   <si>
+    <t>Onderwerp</t>
+  </si>
+  <si>
+    <t>Afzender</t>
+  </si>
+  <si>
+    <t>Categorie</t>
+  </si>
+  <si>
+    <t>Tijdstip</t>
+  </si>
+  <si>
+    <t>Beantwoord</t>
+  </si>
+  <si>
+    <t>Handmatig opvolgen</t>
+  </si>
+  <si>
+    <t>Automatisch afgehandeld</t>
+  </si>
+  <si>
+    <t>Hergebruikt antwoord</t>
+  </si>
+  <si>
     <t>Testmail #1: Wat zijn jullie openingstijden?</t>
   </si>
   <si>
@@ -71,6 +95,9 @@
   </si>
   <si>
     <t>Testmail #20: Kun je dit bespreken met finance?</t>
+  </si>
+  <si>
+    <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -205,6 +232,30 @@
 Voor een snelle afhandeling van uw verzoek, verzoeken wij u vriendelijk om uw ordernummer en reden van retournering te vermelden in uw bericht naar onze klantenservice.
 Met vriendelijke groet,
 [Naam Bedrijf] E-mailassistent</t>
+  </si>
+  <si>
+    <t>Geachte afzender,
+Dank u voor uw e-mail. Helaas kunnen we geen bestellingen plaatsen via deze e-mail. Gelieve onze website te bezoeken en het bestelproces te doorlopen om uw M5-bouten te bestellen.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+  </si>
+  <si>
+    <t>Wil je 100 stuks M5-bouten bestellen?</t>
+  </si>
+  <si>
+    <t>mailmind.test@zohomail.eu</t>
+  </si>
+  <si>
+    <t>Bestelling / Levering</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:35:19</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nee</t>
   </si>
 </sst>
 </file>
@@ -562,162 +613,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:37:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Inhoud</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
+  </si>
+  <si>
+    <t>Testmail #5: Wil je deze klant bellen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -240,16 +243,31 @@
 [E-mailassistent]</t>
   </si>
   <si>
+    <t>Geachte afzender,
+Dank voor uw e-mail. Om u beter van dienst te kunnen zijn, zouden we graag wat meer details ontvangen over welke klant we dienen te benaderen en waarvoor. Kunt u ons de naam van de klant en de reden voor het contact geven? Op die manier kunnen we dit efficiënt afhandelen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
+    <t>Wil je deze klant bellen?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
     <t>Bestelling / Levering</t>
   </si>
   <si>
+    <t>Intern verzoek / Actie voor medewerker</t>
+  </si>
+  <si>
     <t>2025-07-29 21:35:19</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:37:31</t>
   </si>
   <si>
     <t>Ja</t>
@@ -613,7 +631,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -656,7 +674,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -664,7 +682,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -672,7 +690,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -680,7 +698,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -688,7 +706,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -696,7 +714,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -704,7 +722,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -712,7 +730,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -720,7 +738,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -728,7 +746,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -736,7 +754,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -744,7 +762,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -752,7 +770,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -760,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -768,7 +786,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -776,7 +794,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -784,7 +802,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -792,7 +810,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -800,31 +818,63 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="E20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="C21" t="s">
         <v>50</v>
       </c>
-      <c r="G20" t="s">
+      <c r="D21" t="s">
         <v>51</v>
       </c>
-      <c r="H20" t="s">
-        <v>52</v>
-      </c>
-      <c r="I20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" t="s">
-        <v>52</v>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:39:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Inhoud</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Testmail #5: Wil je deze klant bellen?</t>
+  </si>
+  <si>
+    <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -249,12 +252,23 @@
 [Bedrijfsnaam] E-mailassistent</t>
   </si>
   <si>
+    <t>Beste afzender,
+Hartelijk dank voor uw interesse in onze EcoPro-700. Op dit moment hebben we nog voldoende EcoPro-700 op voorraad. U kunt deze direct bestellen via onze website of neem contact met ons op als u meer informatie wenst.
+Met vriendelijke groet,
+[Naam]  
+E-mailassistent  
+[Bedrijfsnaam]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
     <t>Wil je deze klant bellen?</t>
   </si>
   <si>
+    <t>Hebben we EcoPro-700 nog op voorraad?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -264,10 +278,16 @@
     <t>Intern verzoek / Actie voor medewerker</t>
   </si>
   <si>
+    <t>Productinformatie</t>
+  </si>
+  <si>
     <t>2025-07-29 21:35:19</t>
   </si>
   <si>
     <t>2025-07-29 21:37:31</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:39:42</t>
   </si>
   <si>
     <t>Ja</t>
@@ -631,7 +651,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -674,7 +694,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -682,7 +702,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -690,7 +710,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -698,7 +718,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -706,7 +726,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -714,7 +734,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -722,7 +742,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -730,7 +750,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -738,7 +758,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -746,7 +766,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -754,7 +774,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -762,7 +782,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -770,7 +790,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -778,7 +798,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -786,7 +806,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -794,7 +814,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -802,7 +822,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -810,7 +830,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -818,31 +838,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H20" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -850,31 +870,63 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
         <v>50</v>
       </c>
-      <c r="D21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
         <v>53</v>
       </c>
-      <c r="F21" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" t="s">
         <v>57</v>
       </c>
-      <c r="I21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" t="s">
-        <v>57</v>
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:44:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Inhoud</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+  </si>
+  <si>
+    <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -260,6 +263,12 @@
 [Bedrijfsnaam]</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u ons kunnen voorzien van het specifieke product of de service waarover u informatie wenst over de leverbaarheid? Met deze informatie kunnen we gerichter voor u nagaan of het nog leverbaar is.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -269,6 +278,9 @@
     <t>Hebben we EcoPro-700 nog op voorraad?</t>
   </si>
   <si>
+    <t>Kun je nagaan of dit nog leverbaar is?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -288,6 +300,9 @@
   </si>
   <si>
     <t>2025-07-29 21:39:42</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:44:05</t>
   </si>
   <si>
     <t>Ja</t>
@@ -651,7 +666,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -694,7 +709,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -702,7 +717,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -710,7 +725,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -718,7 +733,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -726,7 +741,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -734,7 +749,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -742,7 +757,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -750,7 +765,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -758,7 +773,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -766,7 +781,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -774,7 +789,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -782,7 +797,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -790,7 +805,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -798,7 +813,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -806,7 +821,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -814,7 +829,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -822,7 +837,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -830,7 +845,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -838,31 +853,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="J20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -870,31 +885,31 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H21" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I21" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="J21" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -902,31 +917,63 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
         <v>57</v>
       </c>
-      <c r="F22" t="s">
+      <c r="E23" t="s">
         <v>60</v>
       </c>
-      <c r="G22" t="s">
-        <v>61</v>
-      </c>
-      <c r="H22" t="s">
-        <v>62</v>
-      </c>
-      <c r="I22" t="s">
-        <v>61</v>
-      </c>
-      <c r="J22" t="s">
-        <v>62</v>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" t="s">
+        <v>66</v>
+      </c>
+      <c r="I23" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:51:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>Inhoud</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
+  </si>
+  <si>
+    <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -269,6 +272,13 @@
 [Naam bedrijf]</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor je bericht. Het spijt me te horen dat je retour nog niet is verwerkt. Om dit verder te kunnen onderzoeken, heb ik wat meer informatie van je nodig. Zou je alsjeblieft je ordernummer en/of het trackingnummer van de retourzending kunnen doorgeven? Hiermee kunnen we precies nakijken wat er gaande is en je zo snel mogelijk helpen.
+Met vriendelijke groet,
+[Naam]
+Klantenservice Team</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -281,6 +291,9 @@
     <t>Kun je nagaan of dit nog leverbaar is?</t>
   </si>
   <si>
+    <t>Mijn retour is nog steeds niet verwerkt.</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -293,6 +306,9 @@
     <t>Productinformatie</t>
   </si>
   <si>
+    <t>Retour / Terugbetaling</t>
+  </si>
+  <si>
     <t>2025-07-29 21:35:19</t>
   </si>
   <si>
@@ -303,6 +319,9 @@
   </si>
   <si>
     <t>2025-07-29 21:44:05</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:51:07</t>
   </si>
   <si>
     <t>Ja</t>
@@ -666,7 +685,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -709,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -717,7 +736,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -725,7 +744,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -733,7 +752,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -741,7 +760,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -749,7 +768,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -757,7 +776,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -765,7 +784,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -773,7 +792,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -781,7 +800,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -789,7 +808,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -797,7 +816,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -805,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -813,7 +832,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -821,7 +840,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -829,7 +848,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -837,7 +856,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -845,7 +864,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -853,31 +872,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I20" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J20" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -885,31 +904,31 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J21" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -917,31 +936,31 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H22" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I22" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J22" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -949,31 +968,63 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
         <v>60</v>
       </c>
-      <c r="F23" t="s">
+      <c r="E24" t="s">
         <v>64</v>
       </c>
-      <c r="G23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J23" t="s">
-        <v>66</v>
+      <c r="F24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:53:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>Inhoud</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
+  </si>
+  <si>
+    <t>Testmail #12: Ik heb nog geen geld terug.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -279,6 +282,14 @@
 Klantenservice Team</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor uw e-mail. Om uw vraag beter te kunnen begrijpen en u verder te kunnen helpen, zou ik graag wat meer informatie ontvangen. Kunt u mij uw ordernummer of referentienummer doorgeven, zodat ik kan controleren wat de status is van uw terugbetaling?
+Ik kijk uit naar uw reactie.
+Met vriendelijke groet,
+[Naam] E-mailassistent 
+[Bedrijfsnaam]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -294,6 +305,9 @@
     <t>Mijn retour is nog steeds niet verwerkt.</t>
   </si>
   <si>
+    <t>Ik heb nog geen geld terug.</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -322,6 +336,9 @@
   </si>
   <si>
     <t>2025-07-29 21:51:07</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:53:18</t>
   </si>
   <si>
     <t>Ja</t>
@@ -685,7 +702,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -728,7 +745,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -736,7 +753,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -744,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -752,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -760,7 +777,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -768,7 +785,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -776,7 +793,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -784,7 +801,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -792,7 +809,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -800,7 +817,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -808,7 +825,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -816,7 +833,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -824,7 +841,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -832,7 +849,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -840,7 +857,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -848,7 +865,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -856,7 +873,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -864,7 +881,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -872,31 +889,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I20" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="J20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -904,31 +921,31 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H21" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I21" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="J21" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -936,31 +953,31 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="J22" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -968,31 +985,31 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G23" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I23" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="J23" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1000,31 +1017,63 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H24" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I24" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="J24" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:55:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>Inhoud</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Testmail #12: Ik heb nog geen geld terug.</t>
+  </si>
+  <si>
+    <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -290,6 +293,14 @@
 [Bedrijfsnaam]</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor je bericht. Helaas kan ik je momenteel niet de datasheet van de VentiQ-250 sturen, aangezien ik niet beschik over het specifieke materiaal waar je naar vraagt.
+Ik raad je aan om contact op te nemen met onze verkoopafdeling of de klantenservice, zodat zij je verder kunnen helpen met het verkrijgen van de juiste informatie.
+Met vriendelijke groet,
+[Naam]  
+E-mailassistent bij [Bedrijfsnaam]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -308,6 +319,9 @@
     <t>Ik heb nog geen geld terug.</t>
   </si>
   <si>
+    <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -339,6 +353,9 @@
   </si>
   <si>
     <t>2025-07-29 21:53:18</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:55:30</t>
   </si>
   <si>
     <t>Ja</t>
@@ -702,7 +719,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -745,7 +762,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -753,7 +770,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -761,7 +778,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -769,7 +786,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -777,7 +794,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -785,7 +802,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -793,7 +810,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -801,7 +818,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -809,7 +826,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -817,7 +834,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -825,7 +842,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -833,7 +850,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -841,7 +858,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -849,7 +866,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -857,7 +874,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -865,7 +882,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -873,7 +890,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -881,7 +898,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -889,31 +906,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J20" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -921,31 +938,31 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -953,31 +970,31 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F22" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G22" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H22" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I22" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J22" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -985,31 +1002,31 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I23" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J23" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1017,31 +1034,31 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J24" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1049,31 +1066,63 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H25" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I25" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J25" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" t="s">
+        <v>78</v>
+      </c>
+      <c r="J26" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:57:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
   <si>
     <t>Inhoud</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+  </si>
+  <si>
+    <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -301,6 +304,12 @@
 E-mailassistent bij [Bedrijfsnaam]</t>
   </si>
   <si>
+    <t>Beste klant,
+Dank u voor uw e-mail. Wij kunnen u bevestigen dat dit product over de vereiste CE-certificaten beschikt. Mocht u nog verdere vragen hebben of meer informatie nodig hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -322,6 +331,9 @@
     <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
   </si>
   <si>
+    <t>Heb je de CE-certificaten van dit product?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -356,6 +368,9 @@
   </si>
   <si>
     <t>2025-07-29 21:55:30</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:57:40</t>
   </si>
   <si>
     <t>Ja</t>
@@ -719,7 +734,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -762,7 +777,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -770,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -778,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -786,7 +801,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -794,7 +809,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -802,7 +817,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -810,7 +825,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -818,7 +833,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -826,7 +841,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -834,7 +849,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -842,7 +857,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -850,7 +865,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -858,7 +873,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -866,7 +881,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -874,7 +889,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -882,7 +897,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -890,7 +905,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -898,7 +913,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -906,31 +921,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J20" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -938,31 +953,31 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H21" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J21" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -970,31 +985,31 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J22" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1002,31 +1017,31 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J23" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1034,31 +1049,31 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H24" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J24" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1066,31 +1081,31 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G25" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J25" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1098,31 +1113,63 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="F26" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" t="s">
-        <v>79</v>
-      </c>
-      <c r="I26" t="s">
-        <v>78</v>
-      </c>
-      <c r="J26" t="s">
-        <v>79</v>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" t="s">
+        <v>82</v>
+      </c>
+      <c r="J27" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 22:04:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
   <si>
     <t>Inhoud</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
+  </si>
+  <si>
+    <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -310,6 +313,12 @@
 [Naam bedrijf] E-mailassistent</t>
   </si>
   <si>
+    <t>Beste [Naam],
+Bedankt voor je e-mail. Ik heb de demo op vrijdag om 11:00 uur bij Van Dijk ingepland. Mocht er iets wijzigen of als er nog vragen zijn, laat het me gerust weten.
+Met vriendelijke groet,
+[Jouw Naam]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -334,6 +343,9 @@
     <t>Heb je de CE-certificaten van dit product?</t>
   </si>
   <si>
+    <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -349,6 +361,9 @@
     <t>Retour / Terugbetaling</t>
   </si>
   <si>
+    <t>Planning / Afspraak</t>
+  </si>
+  <si>
     <t>2025-07-29 21:35:19</t>
   </si>
   <si>
@@ -371,6 +386,9 @@
   </si>
   <si>
     <t>2025-07-29 21:57:40</t>
+  </si>
+  <si>
+    <t>2025-07-29 22:04:18</t>
   </si>
   <si>
     <t>Ja</t>
@@ -734,7 +752,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -777,7 +795,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -785,7 +803,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -793,7 +811,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -801,7 +819,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -809,7 +827,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -817,7 +835,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -825,7 +843,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -833,7 +851,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -841,7 +859,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -849,7 +867,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -857,7 +875,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -865,7 +883,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -873,7 +891,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -881,7 +899,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -889,7 +907,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -897,7 +915,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -905,7 +923,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -913,7 +931,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -921,31 +939,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -953,31 +971,31 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I21" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -985,31 +1003,31 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H22" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I22" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J22" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1017,31 +1035,31 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I23" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J23" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1049,31 +1067,31 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J24" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1081,31 +1099,31 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F25" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H25" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I25" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J25" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1113,31 +1131,31 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1145,31 +1163,63 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" t="s">
+        <v>87</v>
+      </c>
+      <c r="J27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
         <v>72</v>
       </c>
-      <c r="F27" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" t="s">
-        <v>83</v>
-      </c>
-      <c r="I27" t="s">
-        <v>82</v>
-      </c>
-      <c r="J27" t="s">
-        <v>83</v>
+      <c r="E28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 22:06:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t>Inhoud</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+  </si>
+  <si>
+    <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -319,6 +322,12 @@
 [Jouw Naam]</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor uw e-mail. Het spijt me, maar het lijkt erop dat u per ongeluk een testmail heeft gestuurd. Als u daadwerkelijk 200 stuks M8-bouten RVS wilt bestellen voor Van Dijk, raad ik u aan om contact op te nemen met onze verkoopafdeling via [verkoop@email.com] of telefonisch via [telefoonnummer]. Zij helpen u graag verder met uw bestelling.
+Met vriendelijke groet,
+[Naam] Nederlandse e-mailassistent van &lt;bedrijfsnaam&gt;</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -346,6 +355,9 @@
     <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
   </si>
   <si>
+    <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -389,6 +401,9 @@
   </si>
   <si>
     <t>2025-07-29 22:04:18</t>
+  </si>
+  <si>
+    <t>2025-07-29 22:06:31</t>
   </si>
   <si>
     <t>Ja</t>
@@ -752,7 +767,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -795,7 +810,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -803,7 +818,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -811,7 +826,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -819,7 +834,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -827,7 +842,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -835,7 +850,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -843,7 +858,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -851,7 +866,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -859,7 +874,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -867,7 +882,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -875,7 +890,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -883,7 +898,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -891,7 +906,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -899,7 +914,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -907,7 +922,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -915,7 +930,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -923,7 +938,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -931,7 +946,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -939,31 +954,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G20" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I20" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J20" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -971,31 +986,31 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H21" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I21" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J21" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1003,31 +1018,31 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G22" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H22" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I22" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J22" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1035,31 +1050,31 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I23" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1067,31 +1082,31 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F24" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H24" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I24" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J24" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1099,31 +1114,31 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H25" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I25" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J25" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1131,31 +1146,31 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H26" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I26" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J26" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1163,31 +1178,31 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H27" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I27" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J27" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1195,31 +1210,63 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H28" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J28" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" t="s">
+        <v>92</v>
+      </c>
+      <c r="I29" t="s">
+        <v>91</v>
+      </c>
+      <c r="J29" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:29:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDC7E0A-8E79-4EA5-956B-33546A075539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Inhoud</t>
   </si>
@@ -62,6 +56,9 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
+  </si>
+  <si>
+    <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -100,12 +97,36 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
+  <si>
+    <t>Beste afzender,
+Bedankt voor je e-mail. Helaas kan ik je niet helpen met het plaatsen van bestellingen via e-mail. Je kunt onze webshop bezoeken om de gewenste M5-bouten te bestellen. Mocht je nog vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam] - E-mailassistent</t>
+  </si>
+  <si>
+    <t>Wil je 100 stuks M5-bouten bestellen?</t>
+  </si>
+  <si>
+    <t>mailmind.test@zohomail.eu</t>
+  </si>
+  <si>
+    <t>Bestelling / Levering</t>
+  </si>
+  <si>
+    <t>2025-07-31 21:29:47</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nee</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,25 +185,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +233,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,7 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -289,10 +301,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,28 +476,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="67.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,36 +515,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:34:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Inhoud</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
+  </si>
+  <si>
+    <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -104,16 +107,31 @@
 [Naam] - E-mailassistent</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor uw vraag. Op dit moment hebben we EcoPro-700 niet op voorraad. We verwachten binnenkort nieuwe voorraad binnen te krijgen. Mocht u nog vragen hebben of een pre-order willen plaatsen, neem dan gerust contact met ons op.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
+    <t>Hebben we EcoPro-700 nog op voorraad?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
     <t>Bestelling / Levering</t>
   </si>
   <si>
+    <t>Productinformatie</t>
+  </si>
+  <si>
     <t>2025-07-31 21:29:47</t>
+  </si>
+  <si>
+    <t>2025-07-31 21:34:42</t>
   </si>
   <si>
     <t>Ja</t>
@@ -477,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -520,7 +538,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -528,7 +546,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -536,7 +554,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -544,7 +562,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -552,31 +570,63 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:39:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Inhoud</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+  </si>
+  <si>
+    <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -113,12 +116,21 @@
 [Bedrijfsnaam]</t>
   </si>
   <si>
+    <t>Beste klant,
+Dank voor uw e-mail. Om u beter van dienst te kunnen zijn, heb ik meer specifieke informatie nodig over het product waar u naar informeert. Kunt u ons het productnummer, de naam van het product of enige details geven zodat we het kunnen controleren in ons systeem? 
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
     <t>Hebben we EcoPro-700 nog op voorraad?</t>
   </si>
   <si>
+    <t>Kun je nagaan of dit nog leverbaar is?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -132,6 +144,9 @@
   </si>
   <si>
     <t>2025-07-31 21:34:42</t>
+  </si>
+  <si>
+    <t>2025-07-31 21:39:04</t>
   </si>
   <si>
     <t>Ja</t>
@@ -495,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -538,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -546,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -554,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -562,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -570,31 +585,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -602,31 +617,63 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="H7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:46:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Inhoud</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
+  </si>
+  <si>
+    <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -122,6 +125,12 @@
 [Bedrijfsnaam]</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor je bericht. We begrijpen dat het vervelend is dat je retourzending nog niet verwerkt is. Om je verder te kunnen helpen, ontvangen we graag wat aanvullende informatie zoals het ordernummer van de retourzending. Zodra we deze gegevens hebben, zullen we direct voor je aan de slag gaan om het probleem op te lossen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -131,6 +140,9 @@
     <t>Kun je nagaan of dit nog leverbaar is?</t>
   </si>
   <si>
+    <t>Mijn retour is nog steeds niet verwerkt.</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -140,6 +152,9 @@
     <t>Productinformatie</t>
   </si>
   <si>
+    <t>Retour / Terugbetaling</t>
+  </si>
+  <si>
     <t>2025-07-31 21:29:47</t>
   </si>
   <si>
@@ -147,6 +162,9 @@
   </si>
   <si>
     <t>2025-07-31 21:39:04</t>
+  </si>
+  <si>
+    <t>2025-07-31 21:45:55</t>
   </si>
   <si>
     <t>Ja</t>
@@ -510,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -553,7 +571,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -561,7 +579,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -569,7 +587,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -577,7 +595,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -585,31 +603,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -617,31 +635,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -649,31 +667,63 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:48:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Inhoud</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
+  </si>
+  <si>
+    <t>Testmail #12: Ik heb nog geen geld terug.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -131,6 +134,12 @@
 [Bedrijfsnaam] E-mailassistent</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor uw e-mail. Om uw vraag over het uitblijven van de terugbetaling te kunnen beantwoorden, hebben we wat meer informatie nodig. Kunt u ons alstublieft uw bestelnummer en de datum van de oorspronkelijke aankoop verstrekken? Op die manier kunnen we dit verder voor u onderzoeken en u zo snel mogelijk van dienst zijn.
+Met vriendelijke groet,
+[Bedrijfsnaam] e-mailassistent</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -143,6 +152,9 @@
     <t>Mijn retour is nog steeds niet verwerkt.</t>
   </si>
   <si>
+    <t>Ik heb nog geen geld terug.</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -165,6 +177,9 @@
   </si>
   <si>
     <t>2025-07-31 21:45:55</t>
+  </si>
+  <si>
+    <t>2025-07-31 21:48:06</t>
   </si>
   <si>
     <t>Ja</t>
@@ -528,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -571,7 +586,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -579,7 +594,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -587,7 +602,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -595,7 +610,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -603,31 +618,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -635,31 +650,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -667,31 +682,31 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -699,31 +714,63 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" t="s">
-        <v>39</v>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:50:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>Inhoud</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Testmail #12: Ik heb nog geen geld terug.</t>
+  </si>
+  <si>
+    <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -140,6 +143,13 @@
 [Bedrijfsnaam] e-mailassistent</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor je interesse in de VentiQ-250. Helaas kunnen we op basis van je e-mailadres geen datasheet vinden. Zou je ons kunnen voorzien van meer informatie, zoals je volledige naam, bedrijfsnaam of eventuele andere gegevens waaronder de datasheet geregistreerd staat? Hiermee kunnen we je beter van dienst zijn en de datasheet naar je opsturen.
+Met vriendelijke groet,
+[Jouw naam]
+E-mailassistent</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -155,6 +165,9 @@
     <t>Ik heb nog geen geld terug.</t>
   </si>
   <si>
+    <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -180,6 +193,9 @@
   </si>
   <si>
     <t>2025-07-31 21:48:06</t>
+  </si>
+  <si>
+    <t>2025-07-31 21:50:21</t>
   </si>
   <si>
     <t>Ja</t>
@@ -543,7 +559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -586,7 +602,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -594,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -602,7 +618,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -610,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -618,31 +634,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -650,31 +666,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -682,31 +698,31 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -714,31 +730,31 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -746,31 +762,63 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" t="s">
-        <v>43</v>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:52:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>Inhoud</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+  </si>
+  <si>
+    <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -150,6 +153,13 @@
 E-mailassistent</t>
   </si>
   <si>
+    <t>Geachte klant,
+Dank u voor uw e-mail. Voor het verkrijgen van de CE-certificaten van het product waar u naar vraagt, verzoeken wij u ons het specifieke productnummer of de productnaam te verstrekken. Met deze informatie kunnen wij u de relevante certificaten verstrekken.
+Als u verdere vragen heeft of meer ondersteuning nodig heeft, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam] E-mailassistent - [Bedrijfsnaam]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -168,6 +178,9 @@
     <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
   </si>
   <si>
+    <t>Heb je de CE-certificaten van dit product?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -196,6 +209,9 @@
   </si>
   <si>
     <t>2025-07-31 21:50:21</t>
+  </si>
+  <si>
+    <t>2025-07-31 21:52:33</t>
   </si>
   <si>
     <t>Ja</t>
@@ -559,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -602,7 +618,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -610,7 +626,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -618,7 +634,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -626,7 +642,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -634,31 +650,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -666,31 +682,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -698,31 +714,31 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -730,31 +746,31 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -762,31 +778,31 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -794,31 +810,63 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" t="s">
-        <v>47</v>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:59:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>Inhoud</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
+  </si>
+  <si>
+    <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -160,6 +163,12 @@
 [Naam] E-mailassistent - [Bedrijfsnaam]</t>
   </si>
   <si>
+    <t>Beste,
+Bedank u voor uw e-mail. Ik zal een demo inplannen bij Van Dijk op vrijdag om 11:00 uur. 
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -181,6 +190,9 @@
     <t>Heb je de CE-certificaten van dit product?</t>
   </si>
   <si>
+    <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -193,6 +205,9 @@
     <t>Retour / Terugbetaling</t>
   </si>
   <si>
+    <t>Planning / Afspraak</t>
+  </si>
+  <si>
     <t>2025-07-31 21:29:47</t>
   </si>
   <si>
@@ -212,6 +227,9 @@
   </si>
   <si>
     <t>2025-07-31 21:52:33</t>
+  </si>
+  <si>
+    <t>2025-07-31 21:59:14</t>
   </si>
   <si>
     <t>Ja</t>
@@ -575,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -618,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -626,7 +644,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -634,7 +652,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -642,7 +660,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -650,31 +668,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -682,31 +700,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -714,31 +732,31 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -746,31 +764,31 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -778,31 +796,31 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -810,31 +828,31 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -842,31 +860,63 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c r="F12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" t="s">
-        <v>50</v>
-      </c>
-      <c r="J12" t="s">
-        <v>51</v>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 22:02:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>Inhoud</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+  </si>
+  <si>
+    <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -169,6 +172,13 @@
 [Naam bedrijf]</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor je e-mail. Helaas kan ik je in dit geval niet verder helpen met je bestelling van 200 stuks M8-bouten RVS voor Van Dijk. Ik raad je aan om contact op te nemen met onze verkoopafdeling of een van onze vertegenwoordigers, zodat zij je verder kunnen assisteren met het plaatsen van deze bestelling.
+Mocht je nog andere vragen hebben of hulp nodig hebben, laat het ons gerust weten.
+Met vriendelijke groet,
+[Naam] E-mailassistent bij [Bedrijfsnaam]</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -193,6 +203,9 @@
     <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
   </si>
   <si>
+    <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -230,6 +243,9 @@
   </si>
   <si>
     <t>2025-07-31 21:59:14</t>
+  </si>
+  <si>
+    <t>2025-07-31 22:01:55</t>
   </si>
   <si>
     <t>Ja</t>
@@ -593,7 +609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -636,7 +652,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -644,7 +660,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -652,7 +668,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -660,7 +676,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -668,31 +684,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -700,31 +716,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -732,31 +748,31 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -764,31 +780,31 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -796,31 +812,31 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -828,31 +844,31 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -860,31 +876,31 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -892,31 +908,63 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="F13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" t="s">
-        <v>56</v>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 22:51:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>Inhoud</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+  </si>
+  <si>
+    <t>Testmail #1: Kun jij dit even regelen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -179,6 +182,12 @@
 [Naam] E-mailassistent bij [Bedrijfsnaam]</t>
   </si>
   <si>
+    <t>Beste klant,
+Dank je wel voor je e-mail. Kun je alsjeblieft meer details geven over wat je precies geregeld wilt hebben? Op die manier kan ik je beter helpen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+  </si>
+  <si>
     <t>Wil je 100 stuks M5-bouten bestellen?</t>
   </si>
   <si>
@@ -206,6 +215,9 @@
     <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
   </si>
   <si>
+    <t>Kun jij dit even regelen?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -221,6 +233,9 @@
     <t>Planning / Afspraak</t>
   </si>
   <si>
+    <t>Overig</t>
+  </si>
+  <si>
     <t>2025-07-31 21:29:47</t>
   </si>
   <si>
@@ -246,6 +261,9 @@
   </si>
   <si>
     <t>2025-07-31 22:01:55</t>
+  </si>
+  <si>
+    <t>2025-08-01 22:51:18</t>
   </si>
   <si>
     <t>Ja</t>
@@ -609,7 +627,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -652,7 +670,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -660,7 +678,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -668,7 +686,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -676,7 +694,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -684,31 +702,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -716,31 +734,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -748,31 +766,31 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -780,31 +798,31 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -812,31 +830,31 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -844,31 +862,31 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -876,31 +894,31 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J12" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -908,31 +926,31 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -940,31 +958,63 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:05:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721EFCA9-5324-4A05-AB7C-E9DECDCFBEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Inhoud</t>
   </si>
@@ -56,9 +62,6 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
-  </si>
-  <si>
-    <t>Testmail #1: Kun jij dit even regelen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -97,37 +100,12 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer specifieke informatie kunnen verstrekken over wat u precies geregeld wilt hebben?
-Met vriendelijke groet,
-[Jouw naam]
-E-mailassistent</t>
-  </si>
-  <si>
-    <t>Kun jij dit even regelen?</t>
-  </si>
-  <si>
-    <t>mailmind.test@zohomail.eu</t>
-  </si>
-  <si>
-    <t>Overig</t>
-  </si>
-  <si>
-    <t>2025-08-01 23:01:32</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Nee</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,17 +164,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -234,7 +220,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -268,6 +254,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -302,9 +289,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -477,14 +465,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,68 +509,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:16:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721EFCA9-5324-4A05-AB7C-E9DECDCFBEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Inhoud</t>
   </si>
@@ -62,6 +56,9 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
+  </si>
+  <si>
+    <t>Testmail #1: Kun jij dit even regelen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -100,12 +97,37 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
+  <si>
+    <t>Beste klant,
+Bedankt voor je e-mail. Om je vraag beter te kunnen beantwoorden, heb ik meer details nodig. Kunt u beschrijven waar u specifiek hulp bij nodig heeft? Als u meer informatie geeft, kan ik u beter van dienst zijn.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+  </si>
+  <si>
+    <t>Kun jij dit even regelen?</t>
+  </si>
+  <si>
+    <t>mailmind.test@zohomail.eu</t>
+  </si>
+  <si>
+    <t>Overig</t>
+  </si>
+  <si>
+    <t>2025-08-01 23:16:44</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nee</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,25 +186,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +234,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,7 +268,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -289,10 +302,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,19 +477,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="46.109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,36 +516,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:18:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4404923F-11B1-45E8-856D-B4E9493604DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Inhoud</t>
   </si>
@@ -56,9 +62,6 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
-  </si>
-  <si>
-    <t>Testmail #1: Kun jij dit even regelen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -97,37 +100,12 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor je e-mail. Om je vraag beter te kunnen beantwoorden, heb ik meer details nodig. Kunt u beschrijven waar u specifiek hulp bij nodig heeft? Als u meer informatie geeft, kan ik u beter van dienst zijn.
-Met vriendelijke groet,
-[Naam]
-E-mailassistent</t>
-  </si>
-  <si>
-    <t>Kun jij dit even regelen?</t>
-  </si>
-  <si>
-    <t>mailmind.test@zohomail.eu</t>
-  </si>
-  <si>
-    <t>Overig</t>
-  </si>
-  <si>
-    <t>2025-08-01 23:16:44</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Nee</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,17 +164,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -234,7 +220,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -268,6 +254,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -302,9 +289,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -477,14 +465,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,68 +506,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:43:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4404923F-11B1-45E8-856D-B4E9493604DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34314442-3795-4B65-BBA5-773BD292E491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:09:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34314442-3795-4B65-BBA5-773BD292E491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE2FF0D-5DEA-45E4-96EE-D4DE0C582C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,10 +469,13 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:18:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE2FF0D-5DEA-45E4-96EE-D4DE0C582C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Inhoud</t>
   </si>
@@ -62,6 +56,9 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
+  </si>
+  <si>
+    <t>Testmail #5: Wil je deze klant bellen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -100,12 +97,37 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
+  <si>
+    <t>Beste collega,
+Dank voor het doorsturen van deze testmail. Kun je wat meer context geven over wie deze klant is en waarom we hen zouden moeten bellen? Dan kan ik de juiste acties ondernemen.
+Met vriendelijke groet,
+[Jouw naam]  
+[Jouw functie]</t>
+  </si>
+  <si>
+    <t>Wil je deze klant bellen?</t>
+  </si>
+  <si>
+    <t>mailmind.test@zohomail.eu</t>
+  </si>
+  <si>
+    <t>Klantenservice / Contact</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:18:33</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nee</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,25 +186,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +234,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,7 +268,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -289,10 +302,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,19 +477,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="46.109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,36 +516,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:22:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A3723B-9293-4EB2-ADCE-41C3452185C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Inhoud</t>
   </si>
@@ -56,9 +62,6 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
-  </si>
-  <si>
-    <t>Testmail #5: Wil je deze klant bellen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -97,37 +100,12 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
-  <si>
-    <t>Beste collega,
-Dank voor het doorsturen van deze testmail. Kun je wat meer context geven over wie deze klant is en waarom we hen zouden moeten bellen? Dan kan ik de juiste acties ondernemen.
-Met vriendelijke groet,
-[Jouw naam]  
-[Jouw functie]</t>
-  </si>
-  <si>
-    <t>Wil je deze klant bellen?</t>
-  </si>
-  <si>
-    <t>mailmind.test@zohomail.eu</t>
-  </si>
-  <si>
-    <t>Klantenservice / Contact</t>
-  </si>
-  <si>
-    <t>2025-08-04 20:18:33</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Nee</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,17 +164,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -234,7 +220,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -268,6 +254,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -302,9 +289,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -477,14 +465,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,68 +506,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:36:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A3723B-9293-4EB2-ADCE-41C3452185C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Inhoud</t>
   </si>
@@ -62,6 +56,9 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
+  </si>
+  <si>
+    <t>Testmail #5: Wil je deze klant bellen?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -100,12 +97,36 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
+  <si>
+    <t>Geachte heer/mevrouw,
+Bedankt voor uw e-mail. We zullen de klant zo snel mogelijk contacteren. Mocht u nog meer informatie hebben die u met ons wilt delen, dan horen we dat graag.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+  </si>
+  <si>
+    <t>Wil je deze klant bellen?</t>
+  </si>
+  <si>
+    <t>mailmind.test@zohomail.eu</t>
+  </si>
+  <si>
+    <t>Klantenservice / Contact</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:36:10</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nee</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,25 +185,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +233,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,7 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -289,10 +301,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,16 +476,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,36 +515,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:49:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Inhoud</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Testmail #5: Wil je deze klant bellen?</t>
+  </si>
+  <si>
+    <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -104,16 +107,31 @@
 [Naam bedrijf]</t>
   </si>
   <si>
+    <t>Beste klant,
+Dank u voor uw bericht. Om uw retourzending verder te kunnen onderzoeken, heb ik wat meer informatie nodig. Kunt u alstublieft uw ordernummer en de datum van de retourzending doorgeven? Op die manier kunnen wij u sneller van dienst zijn.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+  </si>
+  <si>
     <t>Wil je deze klant bellen?</t>
   </si>
   <si>
+    <t>Mijn retour is nog steeds niet verwerkt.</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
     <t>Klantenservice / Contact</t>
   </si>
   <si>
+    <t>Retour / Terugbetaling</t>
+  </si>
+  <si>
     <t>2025-08-04 20:36:10</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:49:17</t>
   </si>
   <si>
     <t>Ja</t>
@@ -477,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -520,7 +538,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -528,7 +546,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -536,7 +554,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -544,7 +562,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -552,31 +570,63 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:51:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Inhoud</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
+  </si>
+  <si>
+    <t>Testmail #12: Ik heb nog geen geld terug.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -113,12 +116,23 @@
 [Naam bedrijf] E-mailassistent</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor uw bericht. Om uw terugbetaling te kunnen verwerken, heb ik wat meer informatie nodig. Kunt u mij uw ordernummer of transactiereferentie geven, zodat ik het voor u kan nakijken?
+Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Naam] 
+E-mailassistent</t>
+  </si>
+  <si>
     <t>Wil je deze klant bellen?</t>
   </si>
   <si>
     <t>Mijn retour is nog steeds niet verwerkt.</t>
   </si>
   <si>
+    <t>Ik heb nog geen geld terug.</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -132,6 +146,9 @@
   </si>
   <si>
     <t>2025-08-04 20:49:17</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:51:30</t>
   </si>
   <si>
     <t>Ja</t>
@@ -495,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -538,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -546,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -554,7 +571,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -562,7 +579,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -570,31 +587,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -602,31 +619,63 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="H7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 21:24:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB23FE04-3521-49B9-B456-2580FF01F8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Inhoud</t>
   </si>
@@ -56,15 +62,6 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
-  </si>
-  <si>
-    <t>Testmail #5: Wil je deze klant bellen?</t>
-  </si>
-  <si>
-    <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
-  </si>
-  <si>
-    <t>Testmail #12: Ik heb nog geen geld terug.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -103,65 +100,12 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
-  <si>
-    <t>Geachte heer/mevrouw,
-Bedankt voor uw e-mail. We zullen de klant zo snel mogelijk contacteren. Mocht u nog meer informatie hebben die u met ons wilt delen, dan horen we dat graag.
-Met vriendelijke groet,
-[Naam bedrijf]</t>
-  </si>
-  <si>
-    <t>Beste klant,
-Dank u voor uw bericht. Om uw retourzending verder te kunnen onderzoeken, heb ik wat meer informatie nodig. Kunt u alstublieft uw ordernummer en de datum van de retourzending doorgeven? Op die manier kunnen wij u sneller van dienst zijn.
-Met vriendelijke groet,
-[Naam bedrijf] E-mailassistent</t>
-  </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor uw bericht. Om uw terugbetaling te kunnen verwerken, heb ik wat meer informatie nodig. Kunt u mij uw ordernummer of transactiereferentie geven, zodat ik het voor u kan nakijken?
-Alvast bedankt voor uw medewerking.
-Met vriendelijke groet,
-[Naam] 
-E-mailassistent</t>
-  </si>
-  <si>
-    <t>Wil je deze klant bellen?</t>
-  </si>
-  <si>
-    <t>Mijn retour is nog steeds niet verwerkt.</t>
-  </si>
-  <si>
-    <t>Ik heb nog geen geld terug.</t>
-  </si>
-  <si>
-    <t>mailmind.test@zohomail.eu</t>
-  </si>
-  <si>
-    <t>Klantenservice / Contact</t>
-  </si>
-  <si>
-    <t>Retour / Terugbetaling</t>
-  </si>
-  <si>
-    <t>2025-08-04 20:36:10</t>
-  </si>
-  <si>
-    <t>2025-08-04 20:49:17</t>
-  </si>
-  <si>
-    <t>2025-08-04 20:51:30</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Nee</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,17 +164,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -268,7 +220,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -302,6 +254,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -336,9 +289,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -511,14 +465,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,132 +506,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 16:18:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB23FE04-3521-49B9-B456-2580FF01F8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Inhoud</t>
   </si>
@@ -62,6 +56,9 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
+  </si>
+  <si>
+    <t>Testmail #1: Ik heb nog geen geld terug.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -100,12 +97,38 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
+  <si>
+    <t>Beste klant,
+Bedankt voor uw bericht. Ik begrijp dat u nog geen geld hebt ontvangen en ik help u hier graag mee verder. Om uw vraag goed te kunnen beantwoorden, zou ik wat meer informatie nodig hebben. Kunt u mij laten weten om welke transactie het gaat en eventueel het bijbehorende referentienummer? Op die manier kan ik het voor u nakijken en u verder helpen.
+Ik kijk uit naar uw reactie.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+  </si>
+  <si>
+    <t>Ik heb nog geen geld terug.</t>
+  </si>
+  <si>
+    <t>mailmind.test@zohomail.eu</t>
+  </si>
+  <si>
+    <t>Retour / Terugbetaling</t>
+  </si>
+  <si>
+    <t>2025-08-05 16:18:34</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nee</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,25 +187,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +235,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,7 +269,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -289,10 +303,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,16 +478,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,36 +517,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:28:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Inhoud</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Testmail #1: Ik heb nog geen geld terug.</t>
+  </si>
+  <si>
+    <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
   </si>
   <si>
     <t>Beste klant,
@@ -106,9 +109,23 @@
 E-mailassistent</t>
   </si>
   <si>
+    <t>Beste klant,
+Bedankt voor je bericht. Ik begrijp dat je retour nog niet is verwerkt en ik wil je graag helpen om dit op te lossen.
+Om dit verder te onderzoeken, heb ik wat meer informatie nodig. Zou je zo vriendelijk willen zijn om je ordernummer en/of trackingnummer met me te delen? Hiermee kan ik de status van je retour nakijken en je zo goed mogelijk van dienst zijn.
+Ik kijk uit naar je reactie.
+Met vriendelijke groet,
+[Naam van de e-mailassistent]  
+Jamie  
+Nederlandse e-mailassistent  
+[Bedrijfsnaam]</t>
+  </si>
+  <si>
     <t>Ik heb nog geen geld terug.</t>
   </si>
   <si>
+    <t>Mijn retour is nog steeds niet verwerkt.</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
@@ -116,6 +133,9 @@
   </si>
   <si>
     <t>2025-08-05 16:18:34</t>
+  </si>
+  <si>
+    <t>2025-08-05 18:28:24</t>
   </si>
   <si>
     <t>Ja</t>
@@ -479,7 +499,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,7 +542,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -530,7 +550,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -538,7 +558,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -546,7 +566,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -554,31 +574,63 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:21:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Inhoud</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
+  </si>
+  <si>
+    <t>Testmail #1: Zou jij dit even op kunnen pakken?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -120,22 +123,37 @@
 [Bedrijfsnaam]</t>
   </si>
   <si>
+    <t>Geachte afzender,
+Dank u voor uw bericht. Kunt u meer details geven over wat u precies wilt dat we oppakken? Zo kunnen we u beter van dienst zijn.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+  </si>
+  <si>
     <t>Ik heb nog geen geld terug.</t>
   </si>
   <si>
     <t>Mijn retour is nog steeds niet verwerkt.</t>
   </si>
   <si>
+    <t>Zou jij dit even op kunnen pakken?</t>
+  </si>
+  <si>
     <t>mailmind.test@zohomail.eu</t>
   </si>
   <si>
     <t>Retour / Terugbetaling</t>
   </si>
   <si>
+    <t>Overig</t>
+  </si>
+  <si>
     <t>2025-08-05 16:18:34</t>
   </si>
   <si>
     <t>2025-08-05 18:28:24</t>
+  </si>
+  <si>
+    <t>2025-08-05 19:21:21</t>
   </si>
   <si>
     <t>Ja</t>
@@ -499,7 +517,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -542,7 +560,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -550,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -558,7 +576,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -566,7 +584,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -574,31 +592,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -606,31 +624,63 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s">
-        <v>29</v>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:27:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A38C08B-C92A-43AE-881F-F7A85A1E1A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Inhoud</t>
   </si>
@@ -56,15 +62,6 @@
   </si>
   <si>
     <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
-  </si>
-  <si>
-    <t>Testmail #1: Ik heb nog geen geld terug.</t>
-  </si>
-  <si>
-    <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
-  </si>
-  <si>
-    <t>Testmail #1: Zou jij dit even op kunnen pakken?</t>
   </si>
   <si>
     <t>Beste klant,
@@ -103,70 +100,12 @@
 Klantenservice Team
 [Bedrijfsnaam]</t>
   </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor uw bericht. Ik begrijp dat u nog geen geld hebt ontvangen en ik help u hier graag mee verder. Om uw vraag goed te kunnen beantwoorden, zou ik wat meer informatie nodig hebben. Kunt u mij laten weten om welke transactie het gaat en eventueel het bijbehorende referentienummer? Op die manier kan ik het voor u nakijken en u verder helpen.
-Ik kijk uit naar uw reactie.
-Met vriendelijke groet,
-[Naam]
-E-mailassistent</t>
-  </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor je bericht. Ik begrijp dat je retour nog niet is verwerkt en ik wil je graag helpen om dit op te lossen.
-Om dit verder te onderzoeken, heb ik wat meer informatie nodig. Zou je zo vriendelijk willen zijn om je ordernummer en/of trackingnummer met me te delen? Hiermee kan ik de status van je retour nakijken en je zo goed mogelijk van dienst zijn.
-Ik kijk uit naar je reactie.
-Met vriendelijke groet,
-[Naam van de e-mailassistent]  
-Jamie  
-Nederlandse e-mailassistent  
-[Bedrijfsnaam]</t>
-  </si>
-  <si>
-    <t>Geachte afzender,
-Dank u voor uw bericht. Kunt u meer details geven over wat u precies wilt dat we oppakken? Zo kunnen we u beter van dienst zijn.
-Met vriendelijke groet,
-[Naam van het bedrijf]</t>
-  </si>
-  <si>
-    <t>Ik heb nog geen geld terug.</t>
-  </si>
-  <si>
-    <t>Mijn retour is nog steeds niet verwerkt.</t>
-  </si>
-  <si>
-    <t>Zou jij dit even op kunnen pakken?</t>
-  </si>
-  <si>
-    <t>mailmind.test@zohomail.eu</t>
-  </si>
-  <si>
-    <t>Retour / Terugbetaling</t>
-  </si>
-  <si>
-    <t>Overig</t>
-  </si>
-  <si>
-    <t>2025-08-05 16:18:34</t>
-  </si>
-  <si>
-    <t>2025-08-05 18:28:24</t>
-  </si>
-  <si>
-    <t>2025-08-05 19:21:21</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Nee</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,17 +164,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -273,7 +220,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -307,6 +254,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -341,9 +289,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -516,14 +465,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,132 +509,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 17:12:50
</commit_message>
<xml_diff>
--- a/logs/historical_responses_cleaned.xlsx
+++ b/logs/historical_responses_cleaned.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MailMind\MailMind\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A38C08B-C92A-43AE-881F-F7A85A1E1A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEB31B7-94F0-4B28-997B-864112976889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Inhoud</t>
   </si>
@@ -50,55 +51,6 @@
   </si>
   <si>
     <t>Hergebruikt antwoord</t>
-  </si>
-  <si>
-    <t>Testmail #4: Ik stuur het pakket terug.</t>
-  </si>
-  <si>
-    <t>Testmail #7: Ik ben niet tevreden met mijn bestelling.</t>
-  </si>
-  <si>
-    <t>Testmail #11: Mijn product is beschadigd geleverd.</t>
-  </si>
-  <si>
-    <t>Testmail #13: Ik wil mijn bestelling ruilen voor maat M.</t>
-  </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor uw bericht. Om uw retourzending zo soepel mogelijk te laten verlopen, vragen wij u vriendelijk om het volgende te doen:
-- Vul het retourformulier in dat bij uw bestelling zat en voeg dit toe aan het pakket.
-- Stuur het pakket terug naar het volgende adres: [adres retourzending].
-- Zodra wij uw retourzending hebben ontvangen, zullen wij het verder afhandelen en u op de hoogte houden van de status van uw retour.
-Mocht u nog verdere vragen of opmerkingen hebben, aarzel dan niet om contact met ons op te nemen.
-Met vriendelijke groet,
-[Naam bedrijf] E-mailassistent</t>
-  </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor uw bericht. Wat vervelend om te horen dat u niet tevreden bent met uw bestelling. Om u beter van dienst te kunnen zijn, zou ik graag meer details willen weten over wat er precies niet naar wens is gegaan. Kunt u mogelijk informatie geven over het specifieke product of de reden waarom u niet tevreden bent? Op die manier kunnen we het probleem verder onderzoeken en een passende oplossing bieden.
-Alvast bedankt voor uw medewerking.
-Met vriendelijke groet,
-[Naam]  
-E-mailassistent  
-[Bedrijfsnaam]</t>
-  </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor het melden van dit probleem. Om u beter van dienst te kunnen zijn, hebben wij wat meer informatie nodig over de beschadiging. Kunt u alstublieft een foto van het beschadigde product meesturen? Dit helpt ons om het probleem beter te begrijpen en een passende oplossing voor u te vinden.
-Met vriendelijke groet,
-[E-mailassistent] van [Bedrijfsnaam]</t>
-  </si>
-  <si>
-    <t>Beste klant,
-Bedankt voor je e-mail. Om je bestelling te ruilen voor maat M, heb ik wat extra informatie nodig. Zou je alsjeblieft de volgende gegevens kunnen doorgeven:
-- Je bestelnummer?
-- Het artikel dat je wilt ruilen en de maat die je wilt ontvangen?
-- Jouw contactgegevens?
-Zodra we deze informatie hebben ontvangen, zullen we de ruiling voor je regelen. Mocht je nog andere vragen hebben, aarzel dan niet om contact met ons op te nemen.
-Met vriendelijke groet,
-[Naam]
-Klantenservice Team
-[Bedrijfsnaam]</t>
   </si>
 </sst>
 </file>
@@ -466,15 +418,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -509,38 +470,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>